<commit_message>
Add OxygenGenerator x 10/100/1000
</commit_message>
<xml_diff>
--- a/SEModCreateTool/生成.xlsx
+++ b/SEModCreateTool/生成.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9105" yWindow="1620" windowWidth="16935" windowHeight="12630" activeTab="2"/>
+    <workbookView xWindow="9105" yWindow="1620" windowWidth="16935" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Bak" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2 (2)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,6 +971,392 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>199216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="図 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="52367" t="27273" r="18655" b="57407"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="238125"/>
+          <a:ext cx="3072075" cy="913591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>199216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="図 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="52367" t="27273" r="18655" b="57407"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="1905000"/>
+          <a:ext cx="3072075" cy="913591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>199216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="図 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="52367" t="27273" r="18655" b="57407"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="3571875"/>
+          <a:ext cx="3072075" cy="913591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1762125" y="619125"/>
+          <a:ext cx="1485900" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" i="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:innerShdw blurRad="63500" dist="50800">
+                  <a:prstClr val="black">
+                    <a:alpha val="50000"/>
+                  </a:prstClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>x 10</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" i="1">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:innerShdw blurRad="63500" dist="50800">
+                <a:prstClr val="black">
+                  <a:alpha val="50000"/>
+                </a:prstClr>
+              </a:innerShdw>
+            </a:effectLst>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1762125" y="2286000"/>
+          <a:ext cx="1485900" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" i="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:innerShdw blurRad="63500" dist="50800">
+                  <a:prstClr val="black">
+                    <a:alpha val="50000"/>
+                  </a:prstClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>x 100</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" i="1">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:innerShdw blurRad="63500" dist="50800">
+                <a:prstClr val="black">
+                  <a:alpha val="50000"/>
+                </a:prstClr>
+              </a:innerShdw>
+            </a:effectLst>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="テキスト ボックス 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1762125" y="3952875"/>
+          <a:ext cx="1485900" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" i="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:innerShdw blurRad="63500" dist="50800">
+                  <a:prstClr val="black">
+                    <a:alpha val="50000"/>
+                  </a:prstClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>x 1000</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" i="1">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:innerShdw blurRad="63500" dist="50800">
+                <a:prstClr val="black">
+                  <a:alpha val="50000"/>
+                </a:prstClr>
+              </a:innerShdw>
+            </a:effectLst>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -1269,7 +1656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2471,7 +2858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
@@ -2486,4 +2873,25 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.375" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="13" width="3.375" style="13"/>
+    <col min="14" max="14" width="2" style="13" customWidth="1"/>
+    <col min="15" max="16384" width="3.375" style="13"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>